<commit_message>
// Travail sur les religions
</commit_message>
<xml_diff>
--- a/Cultures/Liste des cultures.xlsx
+++ b/Cultures/Liste des cultures.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nehwo\Documents\Git\Lorentis\Cultures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2941B16A-46C2-4155-9F13-7939A1F27E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B38D13D6-F969-4F0B-B157-7555AC97F4C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-16320" yWindow="-6555" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lorentis Cultures 2022-07-09-14" sheetId="1" r:id="rId1"/>
@@ -214,7 +214,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -758,20 +758,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:K11" totalsRowShown="0">
-  <autoFilter ref="A1:K11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:K11" totalsRowShown="0">
+  <autoFilter ref="A1:K11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K11">
+    <sortCondition ref="A1:A11"/>
+  </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" name="Id"/>
-    <tableColumn id="2" name="Name" dataDxfId="0"/>
-    <tableColumn id="3" name="Color"/>
-    <tableColumn id="4" name="Cells"/>
-    <tableColumn id="5" name="Expansionism"/>
-    <tableColumn id="6" name="Type"/>
-    <tableColumn id="7" name="Area km2"/>
-    <tableColumn id="8" name="Population"/>
-    <tableColumn id="9" name="Namesbase"/>
-    <tableColumn id="10" name="Emblems Shape"/>
-    <tableColumn id="11" name="Origins"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Color"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Cells"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Expansionism"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Type"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Area km2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Population"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Namesbase"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Emblems Shape"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Origins"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1073,11 +1076,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,238 +1130,226 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="D2">
-        <v>176</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
+        <v>361</v>
       </c>
       <c r="G2">
-        <v>108156</v>
+        <v>244476</v>
       </c>
       <c r="H2">
-        <v>18110981</v>
+        <v>103327</v>
       </c>
       <c r="I2" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="D3">
-        <v>1000</v>
+        <v>333</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G3">
-        <v>493516</v>
+        <v>211548</v>
       </c>
       <c r="H3">
-        <v>13909247</v>
+        <v>6140351</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="J3" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="K3" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D4">
-        <v>832</v>
+        <v>824</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="G4">
-        <v>519096</v>
+        <v>525120</v>
       </c>
       <c r="H4">
-        <v>10483284</v>
+        <v>9690291</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J4" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="K4" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="D5">
-        <v>824</v>
+        <v>485</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="G5">
-        <v>525120</v>
+        <v>309316</v>
       </c>
       <c r="H5">
-        <v>9690291</v>
+        <v>3556666</v>
       </c>
       <c r="I5" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="J5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K5" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="D6">
-        <v>333</v>
+        <v>1000</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="G6">
-        <v>211548</v>
+        <v>493516</v>
       </c>
       <c r="H6">
-        <v>6140351</v>
+        <v>13909247</v>
       </c>
       <c r="I6" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="J6" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="K6" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="D7">
-        <v>397</v>
+        <v>176</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
         <v>14</v>
       </c>
       <c r="G7">
-        <v>252992</v>
+        <v>108156</v>
       </c>
       <c r="H7">
-        <v>5211537</v>
+        <v>18110981</v>
       </c>
       <c r="I7" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="J7" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D8">
-        <v>295</v>
+        <v>397</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F8" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="G8">
-        <v>194300</v>
+        <v>252992</v>
       </c>
       <c r="H8">
-        <v>5136882</v>
+        <v>5211537</v>
       </c>
       <c r="I8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1398,57 +1389,69 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D10">
-        <v>485</v>
+        <v>295</v>
       </c>
       <c r="E10" t="s">
         <v>46</v>
       </c>
       <c r="F10" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="G10">
-        <v>309316</v>
+        <v>194300</v>
       </c>
       <c r="H10">
-        <v>3556666</v>
+        <v>5136882</v>
       </c>
       <c r="I10" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="J10" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>60</v>
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
       </c>
       <c r="D11">
-        <v>361</v>
+        <v>832</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
       </c>
       <c r="G11">
-        <v>244476</v>
+        <v>519096</v>
       </c>
       <c r="H11">
-        <v>103327</v>
+        <v>10483284</v>
       </c>
       <c r="I11" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="J11" t="s">
-        <v>62</v>
+        <v>27</v>
+      </c>
+      <c r="K11" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>